<commit_message>
modified register code file
-- I don't create register for interrupt_CTL and interrupt_ST; but use
process to generate directly the irq signals
</commit_message>
<xml_diff>
--- a/I2C-master/registers/registers.xlsx
+++ b/I2C-master/registers/registers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="102">
   <si>
     <t>CTL</t>
   </si>
@@ -319,6 +319,21 @@
   </si>
   <si>
     <t>RS* = S connect to the STATUS BIT</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>W</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -362,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +426,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -505,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,40 +538,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1513,6 +1534,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E29:K29"/>
+    <mergeCell ref="E24:K24"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="E27:K27"/>
+    <mergeCell ref="E28:K28"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B33:B35"/>
@@ -1529,12 +1556,6 @@
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="D17:K17"/>
     <mergeCell ref="D18:K18"/>
-    <mergeCell ref="E29:K29"/>
-    <mergeCell ref="E24:K24"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="E27:K27"/>
-    <mergeCell ref="E28:K28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1545,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:M27"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1577,7 @@
     <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
@@ -1617,7 +1638,7 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="38" t="s">
         <v>78</v>
       </c>
       <c r="D8" s="30" t="s">
@@ -1634,7 +1655,7 @@
       <c r="M8" s="30"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
+      <c r="B9" s="38"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10">
@@ -1663,7 +1684,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="31">
+      <c r="B10" s="38">
         <v>0</v>
       </c>
       <c r="D10" s="28" t="s">
@@ -1698,7 +1719,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="38"/>
       <c r="D11" s="28"/>
       <c r="E11" s="10" t="s">
         <v>3</v>
@@ -1729,7 +1750,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="38"/>
       <c r="D12" s="28"/>
       <c r="E12" s="10" t="s">
         <v>2</v>
@@ -1760,7 +1781,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="31">
+      <c r="B13" s="38">
         <v>1</v>
       </c>
       <c r="D13" s="28" t="s">
@@ -1793,18 +1814,18 @@
       <c r="M13" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="35" t="s">
+      <c r="P13" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="Q13" s="35"/>
+      <c r="Q13" s="34"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="35" t="s">
+      <c r="S13" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="T13" s="35"/>
+      <c r="T13" s="34"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+      <c r="B14" s="38"/>
       <c r="D14" s="28"/>
       <c r="E14" s="10" t="s">
         <v>3</v>
@@ -1848,7 +1869,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
+      <c r="B15" s="38"/>
       <c r="D15" s="28"/>
       <c r="E15" s="10" t="s">
         <v>2</v>
@@ -1892,25 +1913,25 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="31">
+      <c r="B16" s="38">
         <v>2</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
       <c r="P16" s="17">
         <v>3</v>
       </c>
@@ -1926,21 +1947,21 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="10" t="s">
+      <c r="B17" s="38"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
       <c r="P17" s="17">
         <v>4</v>
       </c>
@@ -1956,21 +1977,21 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="10" t="s">
+      <c r="B18" s="38"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
       <c r="P18" s="17">
         <v>5</v>
       </c>
@@ -1986,25 +2007,25 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="31">
+      <c r="B19" s="38">
         <v>3</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
       <c r="N19" s="7"/>
       <c r="P19" s="17">
         <v>6</v>
@@ -2021,21 +2042,21 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="31"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="10" t="s">
+      <c r="B20" s="38"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
       <c r="P20" s="17">
         <v>7</v>
       </c>
@@ -2051,21 +2072,21 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="10" t="s">
+      <c r="B21" s="38"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
       <c r="P21" s="17">
         <v>8</v>
       </c>
@@ -2081,13 +2102,13 @@
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="31">
+      <c r="B22" s="38">
         <v>4</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="33" t="s">
@@ -2115,9 +2136,9 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="10" t="s">
+      <c r="B23" s="38"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="27" t="s">
         <v>3</v>
       </c>
       <c r="F23" s="33" t="s">
@@ -2145,9 +2166,9 @@
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="10" t="s">
+      <c r="B24" s="38"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="27" t="s">
         <v>2</v>
       </c>
       <c r="F24" s="33" t="s">
@@ -2168,89 +2189,89 @@
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="31">
+      <c r="B25" s="38">
         <v>5</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="G25" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="10" t="s">
+      <c r="B26" s="38"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="27" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
       <c r="U26" s="7"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="10" t="s">
+      <c r="B27" s="38"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="27" t="s">
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
+      <c r="G27" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="31">
+      <c r="B28" s="38">
         <v>6</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="34" t="s">
+      <c r="G28" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
       <c r="P28" s="18"/>
       <c r="Q28" s="18" t="s">
         <v>74</v>
@@ -2262,23 +2283,23 @@
       <c r="U28" s="7"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="31"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="12" t="s">
+      <c r="B29" s="38"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="27" t="s">
         <v>3</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="34" t="s">
+      <c r="G29" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
       <c r="P29" s="18">
         <v>1</v>
       </c>
@@ -2293,23 +2314,23 @@
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="31"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="12" t="s">
+      <c r="B30" s="38"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="27" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="34" t="s">
+      <c r="G30" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
       <c r="P30" s="18">
         <v>2</v>
       </c>
@@ -2324,25 +2345,25 @@
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="31">
+      <c r="B31" s="38">
         <v>7</v>
       </c>
       <c r="D31" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="38" t="s">
+      <c r="F31" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
       <c r="N31" s="13"/>
       <c r="P31" s="18">
         <v>3</v>
@@ -2358,21 +2379,21 @@
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="31"/>
+      <c r="B32" s="38"/>
       <c r="D32" s="36"/>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="38" t="s">
+      <c r="F32" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
       <c r="P32" s="18">
         <v>4</v>
       </c>
@@ -2387,21 +2408,21 @@
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="31"/>
+      <c r="B33" s="38"/>
       <c r="D33" s="36"/>
-      <c r="E33" s="37" t="s">
+      <c r="E33" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="38" t="s">
+      <c r="F33" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
       <c r="P33" s="18">
         <v>5</v>
       </c>
@@ -2416,37 +2437,37 @@
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="31">
+      <c r="B34" s="38">
         <v>8</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="I34" s="15" t="s">
+      <c r="I34" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="J34" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="15" t="s">
+      <c r="K34" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="L34" s="15" t="s">
+      <c r="L34" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="M34" s="15" t="s">
+      <c r="M34" s="39" t="s">
         <v>88</v>
       </c>
       <c r="O34" s="7"/>
@@ -2458,33 +2479,33 @@
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="31"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="42" t="s">
+      <c r="B35" s="38"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="L35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M35" s="15" t="s">
+      <c r="F35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="K35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="39" t="s">
         <v>25</v>
       </c>
       <c r="S35" s="18">
@@ -2495,33 +2516,33 @@
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="31"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="42" t="s">
+      <c r="B36" s="38"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="H36" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="I36" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="J36" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="K36" s="15" t="s">
+      <c r="K36" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="L36" s="15" t="s">
+      <c r="L36" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="M36" s="15" t="s">
+      <c r="M36" s="39" t="s">
         <v>98</v>
       </c>
       <c r="Q36" s="13"/>
@@ -2533,25 +2554,25 @@
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="31">
+      <c r="B37" s="38">
         <v>9</v>
       </c>
       <c r="D37" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="37" t="s">
+      <c r="E37" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="F37" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
       <c r="S37" s="18">
         <v>9</v>
       </c>
@@ -2560,47 +2581,47 @@
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B38" s="31"/>
+      <c r="B38" s="38"/>
       <c r="D38" s="36"/>
-      <c r="E38" s="37" t="s">
+      <c r="E38" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="F38" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="31"/>
+      <c r="B39" s="38"/>
       <c r="D39" s="36"/>
-      <c r="E39" s="37" t="s">
+      <c r="E39" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="39" t="s">
+      <c r="F39" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B40" s="31">
+      <c r="B40" s="38">
         <v>10</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="42" t="s">
         <v>1</v>
       </c>
       <c r="F40" s="40" t="s">
@@ -2629,9 +2650,9 @@
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B41" s="31"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="27" t="s">
+      <c r="B41" s="38"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42" t="s">
         <v>3</v>
       </c>
       <c r="F41" s="40" t="s">
@@ -2660,9 +2681,9 @@
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="31"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="27" t="s">
+      <c r="B42" s="38"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="42" t="s">
         <v>2</v>
       </c>
       <c r="F42" s="40" t="s">
@@ -2691,22 +2712,41 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="H44" s="39" t="s">
+      <c r="H44" s="31" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="H45" s="39"/>
+      <c r="H45" s="31"/>
+      <c r="J45" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F39:M39"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="F31:M31"/>
-    <mergeCell ref="F32:M32"/>
-    <mergeCell ref="F33:M33"/>
-    <mergeCell ref="F37:M37"/>
-    <mergeCell ref="F38:M38"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="F21:M21"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D8:M8"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="F16:M16"/>
+    <mergeCell ref="F17:M17"/>
+    <mergeCell ref="F18:M18"/>
+    <mergeCell ref="F22:M22"/>
+    <mergeCell ref="F23:M23"/>
+    <mergeCell ref="F24:M24"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="S13:T13"/>
@@ -2723,31 +2763,13 @@
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="F19:M19"/>
     <mergeCell ref="F20:M20"/>
-    <mergeCell ref="F21:M21"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D8:M8"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="F16:M16"/>
-    <mergeCell ref="F17:M17"/>
-    <mergeCell ref="F18:M18"/>
-    <mergeCell ref="F22:M22"/>
-    <mergeCell ref="F23:M23"/>
-    <mergeCell ref="F24:M24"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="F39:M39"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="F31:M31"/>
+    <mergeCell ref="F32:M32"/>
+    <mergeCell ref="F33:M33"/>
+    <mergeCell ref="F37:M37"/>
+    <mergeCell ref="F38:M38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>